<commit_message>
more tests on tools
</commit_message>
<xml_diff>
--- a/tools-testing.xlsx
+++ b/tools-testing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>CATEGORIES</t>
   </si>
@@ -278,6 +278,9 @@
       </rPr>
       <t>(Μ.Π.Δ.Σ.),</t>
     </r>
+  </si>
+  <si>
+    <t>respa</t>
   </si>
 </sst>
 </file>
@@ -347,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -371,6 +374,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -944,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:H15"/>
+  <dimension ref="C2:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,20 +965,21 @@
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="37.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="7" max="8" width="37.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D2" s="2" t="s">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
@@ -982,11 +992,14 @@
       <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="3:8" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
@@ -1002,9 +1015,10 @@
       <c r="G4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="3:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="H4" s="10"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="3:9" ht="60" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
@@ -1020,8 +1034,9 @@
       <c r="G5" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="3:9" ht="45" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
@@ -1037,8 +1052,9 @@
       <c r="G6" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="3:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="3:9" ht="90" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1054,8 +1070,9 @@
       <c r="G7" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
         <v>14</v>
       </c>
@@ -1071,8 +1088,9 @@
       <c r="G8" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="3:8" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="3:9" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
@@ -1088,8 +1106,9 @@
       <c r="G9" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1102,8 +1121,9 @@
       <c r="F10" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11" s="4" t="s">
         <v>17</v>
       </c>
@@ -1111,8 +1131,9 @@
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
         <v>32</v>
       </c>
@@ -1120,8 +1141,9 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C13" s="4" t="s">
         <v>34</v>
       </c>
@@ -1137,18 +1159,21 @@
       <c r="G13" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="3:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="H13" s="10"/>
+    </row>
+    <row r="15" spans="3:9" ht="105" x14ac:dyDescent="0.25">
       <c r="F15" s="6" t="s">
         <v>30</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="H15" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D2:H2"/>
+  <mergeCells count="2">
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="H4:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
article parser last paragraph fixes
</commit_message>
<xml_diff>
--- a/tools-testing.xlsx
+++ b/tools-testing.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
   <si>
     <t>CATEGORIES</t>
   </si>
@@ -281,13 +282,494 @@
   </si>
   <si>
     <t>respa</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Οικονομικών </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Π.Δ 142/2017,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Ανάπτυξης και Επενδύσεων </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Π.Δ 5/2022–ΦΕΚ Α' 15/04.02.2022)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Εξωτερικών, Συμβούλιο Απόδημου Ελληνισμού </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ν.4781/2022, ΦΕΚ Α' 31/28.02.2021\</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Εθνικής Άμυνας </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ν. 2292/1995 ΦΕΚ Α'35</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Παιδείας και Θρησκευμάτων </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>π.δ 18/2018 ΦΕΚ Α' 31/23.02.2018</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Εργασίας και Κοινωνικών Υποθέσεων </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>π.δ. 134/2017, ΦΕΚ Α 138/06.11.2017</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Υγείας </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>π.δ. 121/2017, ΦΕΚ Α 1/09.10.2017</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Περιβάλλοντος και Ενέργειας </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>π.δ. 132/2017 ΦΕΚ Α'160/30.10.2017</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Προστασίας του Πολίτη </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ΠΔ 62/2019</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Πολιτισμού και Αθλητισμού </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>π.δ. 4/2018 , ΦΕΚ Α 7/22.01.2018</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Δικαιοσύνης </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>π.δ. 6/2021, ΦΕΚ 7 Α΄/2021</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Εσωτερικών </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Π.Δ 141/2017 - ΦΕΚ 180/Α/23-11-2017</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Μετανάστευσης και Ασύλου </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>π.δ 106/2020,  ΦΕΚ 255/Α/23-12-2020</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Ψηφιακής Διακυβέρνησης </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>π.δ. 40/2020 ΦΕΚ 85/Α/15-4-2020</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Υποδομών και Μεταφορών </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>π.δ. 123/2017 ΦΕΚ Α'151/12.10.2017</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Ναυτιλίας και Νησιωτικής Πολιτικής </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>π.δ. 13/2018, ΦΕΚ Α 26/20.2.2018</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Αγροτικής Ανάπτυξης και Τροφίμων </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>π.δ. 138/2018 ΦΕΚ Α'138/15.09.2017</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Τουρισμού </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>π.δ. 127/2017, ΦΕΚ Α 157/20.10.2017</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF365F91"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Υπουργείο Κλιματικής Κρίσης και Πολιτικής Προστασίας </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ΠΔ 151/2004</t>
+    </r>
+  </si>
+  <si>
+    <t>Άρθρα</t>
+  </si>
+  <si>
+    <t>86/87 (Χάνει το 79 που είναι μονόστηλο και ανάμεσα σε πίνακες)</t>
+  </si>
+  <si>
+    <t>492/492 (Το τελευταίο έχει πίνακα και κάπως χαλάει)</t>
+  </si>
+  <si>
+    <t>75/75</t>
+  </si>
+  <si>
+    <t>49/49</t>
+  </si>
+  <si>
+    <t>27/27</t>
+  </si>
+  <si>
+    <t>90/90 (Στο 74 έχει πίνακα που επηρεάζει το κείμενο)</t>
+  </si>
+  <si>
+    <t>57/57 (Διάφοροι πίνακες στα τελευταία άρθρα)</t>
+  </si>
+  <si>
+    <t>64/64 (55-56 πίνακες)</t>
+  </si>
+  <si>
+    <t>62/62</t>
+  </si>
+  <si>
+    <t>92/92</t>
+  </si>
+  <si>
+    <t>95/94 (Υπάρχει έξτρα Άρθρο *5α)</t>
+  </si>
+  <si>
+    <t>32/32</t>
+  </si>
+  <si>
+    <t>Παράγραφοι</t>
+  </si>
+  <si>
+    <t>*Γενικό σχόλιο: δημιουργείται πρόβλημα όταν υπάρχουν πίνακες</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,8 +805,21 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF365F91"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,6 +829,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -350,7 +851,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -379,6 +880,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -955,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,4 +1686,243 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D1:G22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="85.5703125" customWidth="1"/>
+    <col min="6" max="6" width="59.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="4:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
getting close to mvp
</commit_message>
<xml_diff>
--- a/tools-testing.xlsx
+++ b/tools-testing.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="101">
   <si>
     <t>CATEGORIES</t>
   </si>
@@ -763,6 +764,93 @@
   </si>
   <si>
     <t>*Γενικό σχόλιο: δημιουργείται πρόβλημα όταν υπάρχουν πίνακες</t>
+  </si>
+  <si>
+    <t>α</t>
+  </si>
+  <si>
+    <t>β</t>
+  </si>
+  <si>
+    <t>γ</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t>a line</t>
+  </si>
+  <si>
+    <t>b line</t>
+  </si>
+  <si>
+    <t>aa line</t>
+  </si>
+  <si>
+    <t>1 line</t>
+  </si>
+  <si>
+    <t>2 line</t>
+  </si>
+  <si>
+    <t>bb line</t>
+  </si>
+  <si>
+    <t>3 line</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>Ner</t>
+  </si>
+  <si>
+    <t>Άρθρα 6, 7, 8, 9, 11, 12, 13, 15, 16, 17, 18, 19, 20, 22, 23, 24, 25, 26, 27, 28</t>
+  </si>
+  <si>
+    <t>3.4, INTOSAI  + Άρθρα 24, 56 (2014.)</t>
+  </si>
+  <si>
+    <t>Άρθρα (115 δεν έχει 1.)</t>
+  </si>
+  <si>
+    <t>Άρθρα 11 (το 10 εχει παρενθεση και το χανει) , 14 (ενώνει 1με2 και 3με4 ), 18 (3με4), 63(3με4) {λόγω κενών χαρακτήρων πριν από από τον αριθμό.</t>
+  </si>
+  <si>
+    <t>Άρθρα 9 (3α, β), 13(ξεκιναει με 3α), 20(2με3), 31(ξεκιναει με 3α), 49 προβλημα με αριθμους</t>
+  </si>
+  <si>
+    <t>Προβληματα αριθμων</t>
+  </si>
+  <si>
+    <t>Άρθρα 13, 15-16 (χανει 3α) λογω παρενθεσης), 54, 55</t>
+  </si>
+  <si>
+    <t>Άρθρο 20 μπαχαλο λογω διπλων αρθρων</t>
+  </si>
+  <si>
+    <t>0-1</t>
+  </si>
+  <si>
+    <t>Γενικα το 3α υπαρχει ως 3α, 3.α, 3α), 3α., 3.α., 3 α) Κλπ</t>
+  </si>
+  <si>
+    <t>Άρθρο 16, 25, 80, 87         41-42-52-63-64 (χανει 3α)</t>
+  </si>
+  <si>
+    <t>τα βγαζει ολα ενιαια για δεν χωριζεται με τελειες αλλα με αριθμο)</t>
   </si>
 </sst>
 </file>
@@ -819,7 +907,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -838,8 +926,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -847,11 +947,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -879,13 +1059,63 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1477,14 +1707,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
@@ -1522,7 +1752,7 @@
       <c r="G4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="10"/>
+      <c r="H4" s="22"/>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="3:9" ht="60" x14ac:dyDescent="0.25">
@@ -1541,7 +1771,7 @@
       <c r="G5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="10"/>
+      <c r="H5" s="22"/>
     </row>
     <row r="6" spans="3:9" ht="45" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
@@ -1559,7 +1789,7 @@
       <c r="G6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="10"/>
+      <c r="H6" s="22"/>
     </row>
     <row r="7" spans="3:9" ht="90" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
@@ -1577,7 +1807,7 @@
       <c r="G7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="10"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
@@ -1595,7 +1825,7 @@
       <c r="G8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="10"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="3:9" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
@@ -1613,7 +1843,7 @@
       <c r="G9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="10"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
@@ -1628,7 +1858,7 @@
       <c r="F10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="10"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11" s="4" t="s">
@@ -1638,7 +1868,7 @@
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="10"/>
+      <c r="H11" s="22"/>
     </row>
     <row r="12" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
@@ -1648,7 +1878,7 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="10"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="13" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C13" s="4" t="s">
@@ -1666,7 +1896,7 @@
       <c r="G13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="10"/>
+      <c r="H13" s="22"/>
     </row>
     <row r="15" spans="3:9" ht="105" x14ac:dyDescent="0.25">
       <c r="F15" s="6" t="s">
@@ -1690,235 +1920,756 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:G22"/>
+  <dimension ref="G7:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AA9" sqref="AA9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="7" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>72</v>
+      </c>
+      <c r="O12">
+        <v>3</v>
+      </c>
+      <c r="Q12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>74</v>
+      </c>
+      <c r="N14">
+        <v>4</v>
+      </c>
+      <c r="Q14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+    </row>
+    <row r="17" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>2</v>
+      </c>
+      <c r="P20">
+        <v>3</v>
+      </c>
+      <c r="Q20">
+        <v>4</v>
+      </c>
+      <c r="R20">
+        <v>5</v>
+      </c>
+      <c r="S20">
+        <v>6</v>
+      </c>
+      <c r="T20">
+        <v>7</v>
+      </c>
+      <c r="U20">
+        <v>8</v>
+      </c>
+      <c r="V20">
+        <v>9</v>
+      </c>
+      <c r="W20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="S23" s="12">
+        <v>0</v>
+      </c>
+      <c r="T23" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="U23" s="25"/>
+      <c r="V23" s="25"/>
+    </row>
+    <row r="24" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="N24" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="28"/>
+      <c r="S24" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="28"/>
+    </row>
+    <row r="25" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="N25" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="O25" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="30"/>
+      <c r="S25" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="T25" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="U25" s="29"/>
+      <c r="V25" s="30"/>
+    </row>
+    <row r="26" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="N26" s="14">
+        <v>0</v>
+      </c>
+      <c r="O26" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="24"/>
+      <c r="S26" s="14"/>
+      <c r="T26" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="U26" s="23"/>
+      <c r="V26" s="24"/>
+    </row>
+    <row r="27" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="N27" s="14">
+        <v>0</v>
+      </c>
+      <c r="O27" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="24"/>
+      <c r="S27" s="14"/>
+      <c r="T27" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="U27" s="23"/>
+      <c r="V27" s="24"/>
+    </row>
+    <row r="28" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="N28" s="14">
+        <v>1</v>
+      </c>
+      <c r="O28" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="24"/>
+      <c r="S28" s="14">
+        <v>1</v>
+      </c>
+      <c r="T28" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="U28" s="23"/>
+      <c r="V28" s="24"/>
+    </row>
+    <row r="29" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="N29" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="O29" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="24"/>
+      <c r="S29" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="T29" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="U29" s="23"/>
+      <c r="V29" s="24"/>
+    </row>
+    <row r="30" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="N30" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="O30" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="24"/>
+      <c r="S30" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="T30" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="U30" s="23"/>
+      <c r="V30" s="24"/>
+    </row>
+    <row r="31" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="N31" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="O31" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="P31" s="23"/>
+      <c r="Q31" s="24"/>
+      <c r="S31" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="T31" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="U31" s="23"/>
+      <c r="V31" s="24"/>
+    </row>
+    <row r="32" spans="7:23" x14ac:dyDescent="0.25">
+      <c r="N32" s="14">
+        <v>1</v>
+      </c>
+      <c r="O32" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="24"/>
+      <c r="S32" s="14">
+        <v>1</v>
+      </c>
+      <c r="T32" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="U32" s="23"/>
+      <c r="V32" s="24"/>
+    </row>
+    <row r="33" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N33" s="14">
+        <v>2</v>
+      </c>
+      <c r="O33" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="24"/>
+      <c r="S33" s="14">
+        <v>2</v>
+      </c>
+      <c r="T33" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="U33" s="23"/>
+      <c r="V33" s="24"/>
+    </row>
+    <row r="34" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N34" s="14"/>
+      <c r="O34" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="P34" s="23"/>
+      <c r="Q34" s="24"/>
+      <c r="S34" s="14"/>
+      <c r="T34" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="U34" s="23"/>
+      <c r="V34" s="24"/>
+    </row>
+    <row r="35" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N35" s="14"/>
+      <c r="O35" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="P35" s="23"/>
+      <c r="Q35" s="24"/>
+      <c r="S35" s="14"/>
+      <c r="T35" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="U35" s="23"/>
+      <c r="V35" s="24"/>
+    </row>
+    <row r="36" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N36" s="14"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="16"/>
+      <c r="S36" s="14"/>
+      <c r="T36" s="15"/>
+      <c r="U36" s="15"/>
+      <c r="V36" s="16"/>
+    </row>
+    <row r="37" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N37" s="14"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="16"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="15"/>
+      <c r="V37" s="16"/>
+    </row>
+    <row r="38" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N38" s="14"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="16"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="15"/>
+      <c r="U38" s="15"/>
+      <c r="V38" s="16"/>
+    </row>
+    <row r="39" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N39" s="20"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
+      <c r="Q39" s="18"/>
+      <c r="S39" s="20"/>
+      <c r="T39" s="17"/>
+      <c r="U39" s="17"/>
+      <c r="V39" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="O25:Q25"/>
+    <mergeCell ref="O26:Q26"/>
+    <mergeCell ref="O27:Q27"/>
+    <mergeCell ref="O29:Q29"/>
+    <mergeCell ref="O35:Q35"/>
+    <mergeCell ref="O28:Q28"/>
+    <mergeCell ref="S24:V24"/>
+    <mergeCell ref="T25:V25"/>
+    <mergeCell ref="T26:V26"/>
+    <mergeCell ref="T27:V27"/>
+    <mergeCell ref="T28:V28"/>
+    <mergeCell ref="T29:V29"/>
+    <mergeCell ref="T30:V30"/>
+    <mergeCell ref="T31:V31"/>
+    <mergeCell ref="O30:Q30"/>
+    <mergeCell ref="O31:Q31"/>
+    <mergeCell ref="O32:Q32"/>
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="O33:Q33"/>
+    <mergeCell ref="N24:Q24"/>
+    <mergeCell ref="T32:V32"/>
+    <mergeCell ref="T33:V33"/>
+    <mergeCell ref="T34:V34"/>
+    <mergeCell ref="T35:V35"/>
+    <mergeCell ref="T23:V23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="85.5703125" customWidth="1"/>
     <col min="6" max="6" width="59.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="62.28515625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="54.140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="9" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>38</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>39</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="4:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="31"/>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="4:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="4:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>5</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>42</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>6</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>43</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>7</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>44</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>8</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>45</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>9</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>46</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>10</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>47</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>11</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>48</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>12</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>49</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>13</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>14</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="10" t="s">
         <v>51</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>15</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>52</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>16</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>53</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D18">
         <v>17</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>54</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>18</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="31"/>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>19</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F22" s="4" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="G24" s="9" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>